<commit_message>
modificar campo biddercommission en excel
</commit_message>
<xml_diff>
--- a/public/themes_admin/porto/assets/files/plantillaejemplo.xlsx
+++ b/public/themes_admin/porto/assets/files/plantillaejemplo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\subastas\public\themes_admin\porto\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\subastas\public\themes_admin\porto\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18512680-2870-4EFD-8AE9-D9056B4D3969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E557B50C-C4B7-411C-B43D-FC438A76DF59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="141">
   <si>
     <t>S</t>
   </si>
@@ -447,6 +447,9 @@
   </si>
   <si>
     <t>Características del lote, las “xxxxx” representan el nombre de la característica, por ejemplo: feature/autor o feature/medidas. Puede haber tantas columnas de características como se deseen y estas se crearan por nombre, por lo que no es lo mismo feature/medida que feature/medidas</t>
+  </si>
+  <si>
+    <t>biddercommission</t>
   </si>
 </sst>
 </file>
@@ -1030,9 +1033,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1070,7 +1073,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1176,7 +1179,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1318,7 +1321,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1328,39 +1331,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK3"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="28.109375" customWidth="1"/>
-    <col min="5" max="5" width="32.5546875" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.44140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" style="1" customWidth="1"/>
-    <col min="14" max="16" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="24" width="18.33203125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="14.33203125" customWidth="1"/>
-    <col min="27" max="27" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.88671875" customWidth="1"/>
-    <col min="32" max="32" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="10.109375" customWidth="1"/>
-    <col min="37" max="37" width="141.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" customWidth="1"/>
+    <col min="2" max="3" width="13.90625" customWidth="1"/>
+    <col min="4" max="4" width="28.08984375" customWidth="1"/>
+    <col min="5" max="5" width="32.54296875" customWidth="1"/>
+    <col min="6" max="6" width="21.453125" customWidth="1"/>
+    <col min="7" max="7" width="12.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.453125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.453125" style="1" customWidth="1"/>
+    <col min="14" max="16" width="18.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="24" width="18.36328125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="14.36328125" customWidth="1"/>
+    <col min="27" max="27" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.90625" customWidth="1"/>
+    <col min="32" max="32" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="10.08984375" customWidth="1"/>
+    <col min="37" max="37" width="141.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -1398,7 +1401,7 @@
         <v>55</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>38</v>
+        <v>140</v>
       </c>
       <c r="N1" s="11" t="s">
         <v>39</v>
@@ -1473,7 +1476,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:37" s="1" customFormat="1" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" s="1" customFormat="1" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
@@ -1586,7 +1589,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
@@ -1715,27 +1718,27 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="B1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.88671875" customWidth="1"/>
+    <col min="1" max="1" width="1.90625" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.88671875" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="1.88671875" customWidth="1"/>
-    <col min="6" max="6" width="67.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="1.88671875" customWidth="1"/>
+    <col min="3" max="3" width="1.90625" customWidth="1"/>
+    <col min="4" max="4" width="23.36328125" customWidth="1"/>
+    <col min="5" max="5" width="1.90625" customWidth="1"/>
+    <col min="6" max="6" width="67.90625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.90625" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="1.88671875" customWidth="1"/>
-    <col min="10" max="10" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="1.88671875" customWidth="1"/>
+    <col min="9" max="9" width="1.90625" customWidth="1"/>
+    <col min="10" max="10" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D2" s="10" t="s">
         <v>137</v>
       </c>
@@ -1744,16 +1747,16 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="8" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="2:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="2:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="2:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="6" t="s">
         <v>134</v>
       </c>
@@ -1774,7 +1777,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B7" s="5">
         <v>1</v>
       </c>
@@ -1791,7 +1794,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="5">
         <v>1</v>
       </c>
@@ -1808,7 +1811,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="5">
         <v>1</v>
       </c>
@@ -1825,7 +1828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="5">
         <v>1</v>
       </c>
@@ -1839,7 +1842,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="5">
         <v>1</v>
       </c>
@@ -1853,7 +1856,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="5"/>
       <c r="D12" t="s">
         <v>7</v>
@@ -1868,7 +1871,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="5"/>
       <c r="D13" t="s">
         <v>123</v>
@@ -1880,7 +1883,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="D14" t="s">
         <v>121</v>
@@ -1892,7 +1895,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="5"/>
       <c r="D15" t="s">
         <v>119</v>
@@ -1904,7 +1907,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B16" s="5"/>
       <c r="D16" t="s">
         <v>117</v>
@@ -1916,7 +1919,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B17" s="5"/>
       <c r="D17" t="s">
         <v>115</v>
@@ -1928,7 +1931,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
       <c r="D18" t="s">
         <v>113</v>
@@ -1940,7 +1943,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B19" s="5"/>
       <c r="D19" t="s">
         <v>111</v>
@@ -1952,7 +1955,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B20" s="5"/>
       <c r="D20" t="s">
         <v>109</v>
@@ -1964,7 +1967,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B21" s="5"/>
       <c r="D21" t="s">
         <v>107</v>
@@ -1976,7 +1979,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B22" s="5">
         <v>1</v>
       </c>
@@ -1993,7 +1996,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B23" s="5"/>
       <c r="D23" t="s">
         <v>9</v>
@@ -2008,7 +2011,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B24" s="5"/>
       <c r="D24" t="s">
         <v>10</v>
@@ -2023,7 +2026,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B25" s="5"/>
       <c r="D25" t="s">
         <v>11</v>
@@ -2038,7 +2041,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B26" s="5"/>
       <c r="D26" s="1" t="s">
         <v>37</v>
@@ -2053,7 +2056,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B27" s="5"/>
       <c r="D27" s="1" t="s">
         <v>55</v>
@@ -2065,7 +2068,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B28" s="5"/>
       <c r="D28" s="1" t="s">
         <v>38</v>
@@ -2080,7 +2083,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B29" s="5"/>
       <c r="D29" s="1" t="s">
         <v>39</v>
@@ -2095,7 +2098,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B30" s="5"/>
       <c r="D30" s="1" t="s">
         <v>40</v>
@@ -2110,7 +2113,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B31" s="5"/>
       <c r="D31" s="1" t="s">
         <v>41</v>
@@ -2125,7 +2128,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B32" s="5"/>
       <c r="D32" s="1" t="s">
         <v>42</v>
@@ -2140,7 +2143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B33" s="5"/>
       <c r="D33" s="1" t="s">
         <v>44</v>
@@ -2155,7 +2158,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B34" s="5"/>
       <c r="D34" s="1" t="s">
         <v>45</v>
@@ -2170,7 +2173,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B35" s="5"/>
       <c r="D35" s="1" t="s">
         <v>47</v>
@@ -2185,7 +2188,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B36" s="5"/>
       <c r="D36" s="1" t="s">
         <v>48</v>
@@ -2200,7 +2203,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B37" s="5"/>
       <c r="D37" s="1" t="s">
         <v>49</v>
@@ -2215,7 +2218,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B38" s="5"/>
       <c r="D38" s="1" t="s">
         <v>50</v>
@@ -2230,7 +2233,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B39" s="5"/>
       <c r="D39" s="1" t="s">
         <v>51</v>
@@ -2245,7 +2248,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B40" s="5"/>
       <c r="D40" t="s">
         <v>12</v>
@@ -2260,7 +2263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B41" s="5"/>
       <c r="D41" t="s">
         <v>13</v>
@@ -2275,7 +2278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B42" s="5"/>
       <c r="D42" t="s">
         <v>14</v>
@@ -2290,7 +2293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B43" s="5"/>
       <c r="D43" t="s">
         <v>15</v>
@@ -2305,7 +2308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B44" s="5"/>
       <c r="D44" t="s">
         <v>16</v>
@@ -2320,7 +2323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B45" s="5"/>
       <c r="D45" t="s">
         <v>17</v>
@@ -2335,7 +2338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B46" s="5"/>
       <c r="D46" t="s">
         <v>18</v>
@@ -2350,7 +2353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B47" s="5"/>
       <c r="D47" t="s">
         <v>52</v>
@@ -2365,7 +2368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B48" s="5"/>
       <c r="D48" t="s">
         <v>78</v>
@@ -2380,7 +2383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B49" s="5"/>
       <c r="D49" t="s">
         <v>76</v>
@@ -2395,7 +2398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B50" s="5"/>
       <c r="D50" t="s">
         <v>73</v>
@@ -2410,7 +2413,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B51" s="5"/>
       <c r="D51" t="s">
         <v>71</v>
@@ -2422,7 +2425,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B52" s="5"/>
       <c r="D52" t="s">
         <v>68</v>
@@ -2431,7 +2434,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="53" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B53" s="5"/>
       <c r="D53" t="s">
         <v>19</v>
@@ -2443,7 +2446,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B54" s="5"/>
       <c r="D54" t="s">
         <v>20</v>
@@ -2455,7 +2458,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B55" s="5"/>
       <c r="D55" t="s">
         <v>21</v>
@@ -2467,7 +2470,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B56" s="5"/>
       <c r="D56" t="s">
         <v>22</v>
@@ -2479,7 +2482,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:10" ht="58" x14ac:dyDescent="0.35">
       <c r="B57" s="5"/>
       <c r="D57" t="s">
         <v>23</v>
@@ -2491,7 +2494,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="2:10" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:10" ht="64.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D58" t="s">
         <v>138</v>
       </c>
@@ -2503,6 +2506,15 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="iconSet" priority="2">
+      <iconSet iconSet="3Symbols2">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B7:B57">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Symbols2" showValue="0">
@@ -2519,15 +2531,6 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="iconSet" priority="2">
-      <iconSet iconSet="3Symbols2">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>